<commit_message>
modif short description bb4de7efd728108522c244227f702f5ec0948140
</commit_message>
<xml_diff>
--- a/ig/sd-update-description-short/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-update-description-short/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-15T14:33:28+00:00</t>
+    <t>2024-02-15T14:37:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1690,7 +1690,7 @@
     <t>ResearchStudy.description</t>
   </si>
   <si>
-    <t>Résumé de l'essai / Summary Results</t>
+    <t>Résumé de l'essai (description, durée de participation à l'essai clinique,etc) / Summary Results</t>
   </si>
   <si>
     <t>A full description of how the study is being conducted.</t>

</xml_diff>